<commit_message>
added tuesday jdbc demo
</commit_message>
<xml_diff>
--- a/Workbook7/DatabaseDesign.xlsx
+++ b/Workbook7/DatabaseDesign.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\yearup-learntocode-demos\Workbook7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F36EF737-60E0-4749-9DFA-889ECA11EFB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C29278A9-EF21-4B2C-8732-59E4021D5017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2325" yWindow="540" windowWidth="34020" windowHeight="13230" activeTab="6" xr2:uid="{AA44A1E0-3690-4A20-BC5C-23CA73C5DB15}"/>
+    <workbookView minimized="1" xWindow="780" yWindow="780" windowWidth="27810" windowHeight="14850" activeTab="5" xr2:uid="{AA44A1E0-3690-4A20-BC5C-23CA73C5DB15}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1439" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1440" uniqueCount="424">
   <si>
     <t>CustomerId</t>
   </si>
@@ -1311,6 +1311,9 @@
   </si>
   <si>
     <t>month_price</t>
+  </si>
+  <si>
+    <t>athlete_id</t>
   </si>
 </sst>
 </file>
@@ -1452,17 +1455,12 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1477,15 +1475,24 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1815,7 +1822,7 @@
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="22.28515625" customWidth="1"/>
     <col min="5" max="5" width="59.42578125" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="31.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
@@ -1867,7 +1874,7 @@
       <c r="E1" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="3" t="s">
         <v>7</v>
       </c>
       <c r="G1" s="4" t="s">
@@ -1911,7 +1918,7 @@
       <c r="E2" t="s">
         <v>250</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" t="s">
         <v>202</v>
       </c>
       <c r="G2" s="2">
@@ -1958,7 +1965,7 @@
       <c r="E3" t="s">
         <v>250</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" t="s">
         <v>202</v>
       </c>
       <c r="G3" s="2">
@@ -2005,7 +2012,7 @@
       <c r="E4" t="s">
         <v>250</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" t="s">
         <v>202</v>
       </c>
       <c r="G4" s="2">
@@ -2052,7 +2059,7 @@
       <c r="E5" t="s">
         <v>250</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" t="s">
         <v>202</v>
       </c>
       <c r="G5" s="2">
@@ -2099,7 +2106,7 @@
       <c r="E6" t="s">
         <v>250</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" t="s">
         <v>202</v>
       </c>
       <c r="G6" s="2">
@@ -2146,7 +2153,7 @@
       <c r="E7" t="s">
         <v>250</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" t="s">
         <v>202</v>
       </c>
       <c r="G7" s="2">
@@ -2193,7 +2200,7 @@
       <c r="E8" t="s">
         <v>250</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" t="s">
         <v>202</v>
       </c>
       <c r="G8" s="2">
@@ -2240,7 +2247,7 @@
       <c r="E9" t="s">
         <v>240</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" t="s">
         <v>140</v>
       </c>
       <c r="G9" s="2">
@@ -2287,7 +2294,7 @@
       <c r="E10" t="s">
         <v>240</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" t="s">
         <v>140</v>
       </c>
       <c r="G10" s="2">
@@ -2334,7 +2341,7 @@
       <c r="E11" t="s">
         <v>235</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" t="s">
         <v>107</v>
       </c>
       <c r="G11" s="2">
@@ -2381,7 +2388,7 @@
       <c r="E12" t="s">
         <v>235</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" t="s">
         <v>107</v>
       </c>
       <c r="G12" s="2">
@@ -2428,7 +2435,7 @@
       <c r="E13" t="s">
         <v>230</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" t="s">
         <v>68</v>
       </c>
       <c r="G13" s="2">
@@ -2475,7 +2482,7 @@
       <c r="E14" t="s">
         <v>230</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" t="s">
         <v>68</v>
       </c>
       <c r="G14" s="2">
@@ -2522,7 +2529,7 @@
       <c r="E15" t="s">
         <v>230</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" t="s">
         <v>68</v>
       </c>
       <c r="G15" s="2">
@@ -2569,7 +2576,7 @@
       <c r="E16" t="s">
         <v>234</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F16" t="s">
         <v>100</v>
       </c>
       <c r="G16" s="2">
@@ -2616,7 +2623,7 @@
       <c r="E17" t="s">
         <v>234</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="F17" t="s">
         <v>100</v>
       </c>
       <c r="G17" s="2">
@@ -2663,7 +2670,7 @@
       <c r="E18" t="s">
         <v>234</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F18" t="s">
         <v>100</v>
       </c>
       <c r="G18" s="2">
@@ -2710,7 +2717,7 @@
       <c r="E19" t="s">
         <v>234</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="F19" t="s">
         <v>100</v>
       </c>
       <c r="G19" s="2">
@@ -2757,7 +2764,7 @@
       <c r="E20" t="s">
         <v>234</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="F20" t="s">
         <v>100</v>
       </c>
       <c r="G20" s="2">
@@ -2804,7 +2811,7 @@
       <c r="E21" t="s">
         <v>234</v>
       </c>
-      <c r="F21" s="6" t="s">
+      <c r="F21" t="s">
         <v>100</v>
       </c>
       <c r="G21" s="2">
@@ -2851,7 +2858,7 @@
       <c r="E22" t="s">
         <v>234</v>
       </c>
-      <c r="F22" s="6" t="s">
+      <c r="F22" t="s">
         <v>100</v>
       </c>
       <c r="G22" s="2">
@@ -2898,7 +2905,7 @@
       <c r="E23" t="s">
         <v>239</v>
       </c>
-      <c r="F23" s="6" t="s">
+      <c r="F23" t="s">
         <v>136</v>
       </c>
       <c r="G23" s="2">
@@ -2945,7 +2952,7 @@
       <c r="E24" t="s">
         <v>239</v>
       </c>
-      <c r="F24" s="6" t="s">
+      <c r="F24" t="s">
         <v>136</v>
       </c>
       <c r="G24" s="2">
@@ -2992,7 +2999,7 @@
       <c r="E25" t="s">
         <v>242</v>
       </c>
-      <c r="F25" s="6" t="s">
+      <c r="F25" t="s">
         <v>152</v>
       </c>
       <c r="G25" s="2">
@@ -3039,7 +3046,7 @@
       <c r="E26" t="s">
         <v>242</v>
       </c>
-      <c r="F26" s="6" t="s">
+      <c r="F26" t="s">
         <v>152</v>
       </c>
       <c r="G26" s="2">
@@ -3086,7 +3093,7 @@
       <c r="E27" t="s">
         <v>242</v>
       </c>
-      <c r="F27" s="6" t="s">
+      <c r="F27" t="s">
         <v>152</v>
       </c>
       <c r="G27" s="2">
@@ -3133,7 +3140,7 @@
       <c r="E28" t="s">
         <v>243</v>
       </c>
-      <c r="F28" s="6" t="s">
+      <c r="F28" t="s">
         <v>159</v>
       </c>
       <c r="G28" s="2">
@@ -3180,7 +3187,7 @@
       <c r="E29" t="s">
         <v>243</v>
       </c>
-      <c r="F29" s="6" t="s">
+      <c r="F29" t="s">
         <v>159</v>
       </c>
       <c r="G29" s="2">
@@ -3227,7 +3234,7 @@
       <c r="E30" t="s">
         <v>227</v>
       </c>
-      <c r="F30" s="6" t="s">
+      <c r="F30" t="s">
         <v>39</v>
       </c>
       <c r="G30" s="2">
@@ -3274,7 +3281,7 @@
       <c r="E31" t="s">
         <v>227</v>
       </c>
-      <c r="F31" s="6" t="s">
+      <c r="F31" t="s">
         <v>39</v>
       </c>
       <c r="G31" s="2">
@@ -3321,7 +3328,7 @@
       <c r="E32" t="s">
         <v>227</v>
       </c>
-      <c r="F32" s="6" t="s">
+      <c r="F32" t="s">
         <v>39</v>
       </c>
       <c r="G32" s="2">
@@ -3368,7 +3375,7 @@
       <c r="E33" t="s">
         <v>227</v>
       </c>
-      <c r="F33" s="6" t="s">
+      <c r="F33" t="s">
         <v>39</v>
       </c>
       <c r="G33" s="2">
@@ -3415,7 +3422,7 @@
       <c r="E34" t="s">
         <v>227</v>
       </c>
-      <c r="F34" s="6" t="s">
+      <c r="F34" t="s">
         <v>39</v>
       </c>
       <c r="G34" s="2">
@@ -3462,7 +3469,7 @@
       <c r="E35" t="s">
         <v>227</v>
       </c>
-      <c r="F35" s="6" t="s">
+      <c r="F35" t="s">
         <v>39</v>
       </c>
       <c r="G35" s="2">
@@ -3509,7 +3516,7 @@
       <c r="E36" t="s">
         <v>233</v>
       </c>
-      <c r="F36" s="6" t="s">
+      <c r="F36" t="s">
         <v>94</v>
       </c>
       <c r="G36" s="2">
@@ -3556,7 +3563,7 @@
       <c r="E37" t="s">
         <v>233</v>
       </c>
-      <c r="F37" s="6" t="s">
+      <c r="F37" t="s">
         <v>94</v>
       </c>
       <c r="G37" s="2">
@@ -3603,7 +3610,7 @@
       <c r="E38" t="s">
         <v>233</v>
       </c>
-      <c r="F38" s="6" t="s">
+      <c r="F38" t="s">
         <v>94</v>
       </c>
       <c r="G38" s="2">
@@ -3650,7 +3657,7 @@
       <c r="E39" t="s">
         <v>251</v>
       </c>
-      <c r="F39" s="6" t="s">
+      <c r="F39" t="s">
         <v>210</v>
       </c>
       <c r="G39" s="2">
@@ -3697,7 +3704,7 @@
       <c r="E40" t="s">
         <v>251</v>
       </c>
-      <c r="F40" s="6" t="s">
+      <c r="F40" t="s">
         <v>210</v>
       </c>
       <c r="G40" s="2">
@@ -3744,7 +3751,7 @@
       <c r="E41" t="s">
         <v>251</v>
       </c>
-      <c r="F41" s="6" t="s">
+      <c r="F41" t="s">
         <v>210</v>
       </c>
       <c r="G41" s="2">
@@ -3791,7 +3798,7 @@
       <c r="E42" t="s">
         <v>251</v>
       </c>
-      <c r="F42" s="6" t="s">
+      <c r="F42" t="s">
         <v>210</v>
       </c>
       <c r="G42" s="2">
@@ -3838,7 +3845,7 @@
       <c r="E43" t="s">
         <v>251</v>
       </c>
-      <c r="F43" s="6" t="s">
+      <c r="F43" t="s">
         <v>210</v>
       </c>
       <c r="G43" s="2">
@@ -3885,7 +3892,7 @@
       <c r="E44" t="s">
         <v>253</v>
       </c>
-      <c r="F44" s="6" t="s">
+      <c r="F44" t="s">
         <v>221</v>
       </c>
       <c r="G44" s="2">
@@ -3932,7 +3939,7 @@
       <c r="E45" t="s">
         <v>253</v>
       </c>
-      <c r="F45" s="6" t="s">
+      <c r="F45" t="s">
         <v>221</v>
       </c>
       <c r="G45" s="2">
@@ -3979,7 +3986,7 @@
       <c r="E46" t="s">
         <v>253</v>
       </c>
-      <c r="F46" s="6" t="s">
+      <c r="F46" t="s">
         <v>221</v>
       </c>
       <c r="G46" s="2">
@@ -4026,7 +4033,7 @@
       <c r="E47" t="s">
         <v>253</v>
       </c>
-      <c r="F47" s="6" t="s">
+      <c r="F47" t="s">
         <v>221</v>
       </c>
       <c r="G47" s="2">
@@ -4073,7 +4080,7 @@
       <c r="E48" t="s">
         <v>247</v>
       </c>
-      <c r="F48" s="6" t="s">
+      <c r="F48" t="s">
         <v>183</v>
       </c>
       <c r="G48" s="2">
@@ -4120,7 +4127,7 @@
       <c r="E49" t="s">
         <v>247</v>
       </c>
-      <c r="F49" s="6" t="s">
+      <c r="F49" t="s">
         <v>183</v>
       </c>
       <c r="G49" s="2">
@@ -4167,7 +4174,7 @@
       <c r="E50" t="s">
         <v>249</v>
       </c>
-      <c r="F50" s="6" t="s">
+      <c r="F50" t="s">
         <v>195</v>
       </c>
       <c r="G50" s="2">
@@ -4214,7 +4221,7 @@
       <c r="E51" t="s">
         <v>249</v>
       </c>
-      <c r="F51" s="6" t="s">
+      <c r="F51" t="s">
         <v>195</v>
       </c>
       <c r="G51" s="2">
@@ -4261,7 +4268,7 @@
       <c r="E52" t="s">
         <v>236</v>
       </c>
-      <c r="F52" s="6" t="s">
+      <c r="F52" t="s">
         <v>114</v>
       </c>
       <c r="G52" s="2">
@@ -4308,7 +4315,7 @@
       <c r="E53" t="s">
         <v>236</v>
       </c>
-      <c r="F53" s="6" t="s">
+      <c r="F53" t="s">
         <v>114</v>
       </c>
       <c r="G53" s="2">
@@ -4355,7 +4362,7 @@
       <c r="E54" t="s">
         <v>236</v>
       </c>
-      <c r="F54" s="6" t="s">
+      <c r="F54" t="s">
         <v>114</v>
       </c>
       <c r="G54" s="2">
@@ -4402,7 +4409,7 @@
       <c r="E55" t="s">
         <v>236</v>
       </c>
-      <c r="F55" s="6" t="s">
+      <c r="F55" t="s">
         <v>114</v>
       </c>
       <c r="G55" s="2">
@@ -4449,7 +4456,7 @@
       <c r="E56" t="s">
         <v>237</v>
       </c>
-      <c r="F56" s="6" t="s">
+      <c r="F56" t="s">
         <v>120</v>
       </c>
       <c r="G56" s="2">
@@ -4496,7 +4503,7 @@
       <c r="E57" t="s">
         <v>237</v>
       </c>
-      <c r="F57" s="6" t="s">
+      <c r="F57" t="s">
         <v>120</v>
       </c>
       <c r="G57" s="2">
@@ -4543,7 +4550,7 @@
       <c r="E58" t="s">
         <v>246</v>
       </c>
-      <c r="F58" s="6" t="s">
+      <c r="F58" t="s">
         <v>176</v>
       </c>
       <c r="G58" s="2">
@@ -4590,7 +4597,7 @@
       <c r="E59" t="s">
         <v>246</v>
       </c>
-      <c r="F59" s="6" t="s">
+      <c r="F59" t="s">
         <v>176</v>
       </c>
       <c r="G59" s="2">
@@ -4637,7 +4644,7 @@
       <c r="E60" t="s">
         <v>246</v>
       </c>
-      <c r="F60" s="6" t="s">
+      <c r="F60" t="s">
         <v>176</v>
       </c>
       <c r="G60" s="2">
@@ -4684,7 +4691,7 @@
       <c r="E61" t="s">
         <v>246</v>
       </c>
-      <c r="F61" s="6" t="s">
+      <c r="F61" t="s">
         <v>176</v>
       </c>
       <c r="G61" s="2">
@@ -4731,7 +4738,7 @@
       <c r="E62" t="s">
         <v>246</v>
       </c>
-      <c r="F62" s="6" t="s">
+      <c r="F62" t="s">
         <v>176</v>
       </c>
       <c r="G62" s="2">
@@ -4778,7 +4785,7 @@
       <c r="E63" t="s">
         <v>246</v>
       </c>
-      <c r="F63" s="6" t="s">
+      <c r="F63" t="s">
         <v>176</v>
       </c>
       <c r="G63" s="2">
@@ -4825,7 +4832,7 @@
       <c r="E64" t="s">
         <v>238</v>
       </c>
-      <c r="F64" s="6" t="s">
+      <c r="F64" t="s">
         <v>128</v>
       </c>
       <c r="G64" s="2">
@@ -4872,7 +4879,7 @@
       <c r="E65" t="s">
         <v>238</v>
       </c>
-      <c r="F65" s="6" t="s">
+      <c r="F65" t="s">
         <v>128</v>
       </c>
       <c r="G65" s="2">
@@ -4919,7 +4926,7 @@
       <c r="E66" t="s">
         <v>238</v>
       </c>
-      <c r="F66" s="6" t="s">
+      <c r="F66" t="s">
         <v>128</v>
       </c>
       <c r="G66" s="2">
@@ -4966,7 +4973,7 @@
       <c r="E67" t="s">
         <v>238</v>
       </c>
-      <c r="F67" s="6" t="s">
+      <c r="F67" t="s">
         <v>128</v>
       </c>
       <c r="G67" s="2">
@@ -5013,7 +5020,7 @@
       <c r="E68" t="s">
         <v>238</v>
       </c>
-      <c r="F68" s="6" t="s">
+      <c r="F68" t="s">
         <v>128</v>
       </c>
       <c r="G68" s="2">
@@ -5060,7 +5067,7 @@
       <c r="E69" t="s">
         <v>238</v>
       </c>
-      <c r="F69" s="6" t="s">
+      <c r="F69" t="s">
         <v>128</v>
       </c>
       <c r="G69" s="2">
@@ -5107,7 +5114,7 @@
       <c r="E70" t="s">
         <v>231</v>
       </c>
-      <c r="F70" s="6" t="s">
+      <c r="F70" t="s">
         <v>78</v>
       </c>
       <c r="G70" s="2">
@@ -5154,7 +5161,7 @@
       <c r="E71" t="s">
         <v>231</v>
       </c>
-      <c r="F71" s="6" t="s">
+      <c r="F71" t="s">
         <v>78</v>
       </c>
       <c r="G71" s="2">
@@ -5201,7 +5208,7 @@
       <c r="E72" t="s">
         <v>231</v>
       </c>
-      <c r="F72" s="6" t="s">
+      <c r="F72" t="s">
         <v>78</v>
       </c>
       <c r="G72" s="2">
@@ -5248,7 +5255,7 @@
       <c r="E73" t="s">
         <v>231</v>
       </c>
-      <c r="F73" s="6" t="s">
+      <c r="F73" t="s">
         <v>78</v>
       </c>
       <c r="G73" s="2">
@@ -5295,7 +5302,7 @@
       <c r="E74" t="s">
         <v>252</v>
       </c>
-      <c r="F74" s="6" t="s">
+      <c r="F74" t="s">
         <v>215</v>
       </c>
       <c r="G74" s="2">
@@ -5342,7 +5349,7 @@
       <c r="E75" t="s">
         <v>252</v>
       </c>
-      <c r="F75" s="6" t="s">
+      <c r="F75" t="s">
         <v>215</v>
       </c>
       <c r="G75" s="2">
@@ -5389,7 +5396,7 @@
       <c r="E76" t="s">
         <v>252</v>
       </c>
-      <c r="F76" s="6" t="s">
+      <c r="F76" t="s">
         <v>215</v>
       </c>
       <c r="G76" s="2">
@@ -5436,7 +5443,7 @@
       <c r="E77" t="s">
         <v>252</v>
       </c>
-      <c r="F77" s="6" t="s">
+      <c r="F77" t="s">
         <v>215</v>
       </c>
       <c r="G77" s="2">
@@ -5483,7 +5490,7 @@
       <c r="E78" t="s">
         <v>252</v>
       </c>
-      <c r="F78" s="6" t="s">
+      <c r="F78" t="s">
         <v>215</v>
       </c>
       <c r="G78" s="2">
@@ -5530,7 +5537,7 @@
       <c r="E79" t="s">
         <v>245</v>
       </c>
-      <c r="F79" s="6" t="s">
+      <c r="F79" t="s">
         <v>171</v>
       </c>
       <c r="G79" s="2">
@@ -5577,7 +5584,7 @@
       <c r="E80" t="s">
         <v>229</v>
       </c>
-      <c r="F80" s="6" t="s">
+      <c r="F80" t="s">
         <v>54</v>
       </c>
       <c r="G80" s="2">
@@ -5624,7 +5631,7 @@
       <c r="E81" t="s">
         <v>229</v>
       </c>
-      <c r="F81" s="6" t="s">
+      <c r="F81" t="s">
         <v>54</v>
       </c>
       <c r="G81" s="2">
@@ -5671,7 +5678,7 @@
       <c r="E82" t="s">
         <v>229</v>
       </c>
-      <c r="F82" s="6" t="s">
+      <c r="F82" t="s">
         <v>54</v>
       </c>
       <c r="G82" s="2">
@@ -5718,7 +5725,7 @@
       <c r="E83" t="s">
         <v>226</v>
       </c>
-      <c r="F83" s="6" t="s">
+      <c r="F83" t="s">
         <v>32</v>
       </c>
       <c r="G83" s="2">
@@ -5765,7 +5772,7 @@
       <c r="E84" t="s">
         <v>226</v>
       </c>
-      <c r="F84" s="6" t="s">
+      <c r="F84" t="s">
         <v>32</v>
       </c>
       <c r="G84" s="2">
@@ -5812,7 +5819,7 @@
       <c r="E85" t="s">
         <v>248</v>
       </c>
-      <c r="F85" s="6" t="s">
+      <c r="F85" t="s">
         <v>188</v>
       </c>
       <c r="G85" s="2">
@@ -5859,7 +5866,7 @@
       <c r="E86" t="s">
         <v>248</v>
       </c>
-      <c r="F86" s="6" t="s">
+      <c r="F86" t="s">
         <v>188</v>
       </c>
       <c r="G86" s="2">
@@ -5906,7 +5913,7 @@
       <c r="E87" t="s">
         <v>228</v>
       </c>
-      <c r="F87" s="6" t="s">
+      <c r="F87" t="s">
         <v>48</v>
       </c>
       <c r="G87" s="2">
@@ -5953,7 +5960,7 @@
       <c r="E88" t="s">
         <v>228</v>
       </c>
-      <c r="F88" s="6" t="s">
+      <c r="F88" t="s">
         <v>48</v>
       </c>
       <c r="G88" s="2">
@@ -6000,7 +6007,7 @@
       <c r="E89" t="s">
         <v>228</v>
       </c>
-      <c r="F89" s="6" t="s">
+      <c r="F89" t="s">
         <v>48</v>
       </c>
       <c r="G89" s="2">
@@ -6047,7 +6054,7 @@
       <c r="E90" t="s">
         <v>225</v>
       </c>
-      <c r="F90" s="6" t="s">
+      <c r="F90" t="s">
         <v>21</v>
       </c>
       <c r="G90" s="2">
@@ -6094,7 +6101,7 @@
       <c r="E91" t="s">
         <v>225</v>
       </c>
-      <c r="F91" s="6" t="s">
+      <c r="F91" t="s">
         <v>21</v>
       </c>
       <c r="G91" s="2">
@@ -6141,7 +6148,7 @@
       <c r="E92" t="s">
         <v>225</v>
       </c>
-      <c r="F92" s="6" t="s">
+      <c r="F92" t="s">
         <v>21</v>
       </c>
       <c r="G92" s="2">
@@ -6188,7 +6195,7 @@
       <c r="E93" t="s">
         <v>225</v>
       </c>
-      <c r="F93" s="6" t="s">
+      <c r="F93" t="s">
         <v>21</v>
       </c>
       <c r="G93" s="2">
@@ -6235,7 +6242,7 @@
       <c r="E94" t="s">
         <v>225</v>
       </c>
-      <c r="F94" s="6" t="s">
+      <c r="F94" t="s">
         <v>21</v>
       </c>
       <c r="G94" s="2">
@@ -6282,7 +6289,7 @@
       <c r="E95" t="s">
         <v>241</v>
       </c>
-      <c r="F95" s="6" t="s">
+      <c r="F95" t="s">
         <v>146</v>
       </c>
       <c r="G95" s="2">
@@ -6329,7 +6336,7 @@
       <c r="E96" t="s">
         <v>241</v>
       </c>
-      <c r="F96" s="6" t="s">
+      <c r="F96" t="s">
         <v>146</v>
       </c>
       <c r="G96" s="2">
@@ -6376,7 +6383,7 @@
       <c r="E97" t="s">
         <v>241</v>
       </c>
-      <c r="F97" s="6" t="s">
+      <c r="F97" t="s">
         <v>146</v>
       </c>
       <c r="G97" s="2">
@@ -6423,7 +6430,7 @@
       <c r="E98" t="s">
         <v>232</v>
       </c>
-      <c r="F98" s="6" t="s">
+      <c r="F98" t="s">
         <v>86</v>
       </c>
       <c r="G98" s="2">
@@ -6470,7 +6477,7 @@
       <c r="E99" t="s">
         <v>232</v>
       </c>
-      <c r="F99" s="6" t="s">
+      <c r="F99" t="s">
         <v>86</v>
       </c>
       <c r="G99" s="2">
@@ -6517,7 +6524,7 @@
       <c r="E100" t="s">
         <v>244</v>
       </c>
-      <c r="F100" s="6" t="s">
+      <c r="F100" t="s">
         <v>165</v>
       </c>
       <c r="G100" s="2">
@@ -6564,7 +6571,7 @@
       <c r="E101" t="s">
         <v>244</v>
       </c>
-      <c r="F101" s="6" t="s">
+      <c r="F101" t="s">
         <v>165</v>
       </c>
       <c r="G101" s="2">
@@ -6614,13 +6621,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.140625" customWidth="1"/>
     <col min="3" max="3" width="18.140625" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
     <col min="5" max="5" width="25.140625" customWidth="1"/>
     <col min="6" max="9" width="19.140625" customWidth="1"/>
-    <col min="10" max="10" width="27.42578125" style="6" customWidth="1"/>
+    <col min="10" max="10" width="27.42578125" customWidth="1"/>
     <col min="11" max="11" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.42578125" bestFit="1" customWidth="1"/>
@@ -6678,12 +6685,12 @@
       <c r="I1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="5" t="s">
         <v>197</v>
       </c>
       <c r="B2" t="s">
@@ -6710,7 +6717,7 @@
       <c r="I2" t="s">
         <v>262</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" t="s">
         <v>202</v>
       </c>
       <c r="K2" s="1"/>
@@ -6718,7 +6725,7 @@
       <c r="M2" s="1"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="5" t="s">
         <v>137</v>
       </c>
       <c r="B3" t="s">
@@ -6745,7 +6752,7 @@
       <c r="I3" t="s">
         <v>266</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" t="s">
         <v>140</v>
       </c>
       <c r="K3" s="1"/>
@@ -6753,7 +6760,7 @@
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="5" t="s">
         <v>103</v>
       </c>
       <c r="B4" t="s">
@@ -6780,7 +6787,7 @@
       <c r="I4" t="s">
         <v>269</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="J4" t="s">
         <v>107</v>
       </c>
       <c r="K4" s="1"/>
@@ -6788,7 +6795,7 @@
       <c r="M4" s="1"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="5" t="s">
         <v>63</v>
       </c>
       <c r="B5" t="s">
@@ -6815,7 +6822,7 @@
       <c r="I5" t="s">
         <v>272</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="J5" t="s">
         <v>68</v>
       </c>
       <c r="K5" s="1"/>
@@ -6823,7 +6830,7 @@
       <c r="M5" s="1"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="5" t="s">
         <v>96</v>
       </c>
       <c r="B6" t="s">
@@ -6850,7 +6857,7 @@
       <c r="I6" t="s">
         <v>275</v>
       </c>
-      <c r="J6" s="6" t="s">
+      <c r="J6" t="s">
         <v>100</v>
       </c>
       <c r="K6" s="1"/>
@@ -6858,7 +6865,7 @@
       <c r="M6" s="1"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="5" t="s">
         <v>132</v>
       </c>
       <c r="B7" t="s">
@@ -6885,7 +6892,7 @@
       <c r="I7" t="s">
         <v>262</v>
       </c>
-      <c r="J7" s="6" t="s">
+      <c r="J7" t="s">
         <v>136</v>
       </c>
       <c r="K7" s="1"/>
@@ -6893,7 +6900,7 @@
       <c r="M7" s="1"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="5" t="s">
         <v>148</v>
       </c>
       <c r="B8" t="s">
@@ -6920,7 +6927,7 @@
       <c r="I8" t="s">
         <v>280</v>
       </c>
-      <c r="J8" s="6" t="s">
+      <c r="J8" t="s">
         <v>152</v>
       </c>
       <c r="K8" s="1"/>
@@ -6928,7 +6935,7 @@
       <c r="M8" s="1"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="5" t="s">
         <v>155</v>
       </c>
       <c r="B9" t="s">
@@ -6955,7 +6962,7 @@
       <c r="I9" t="s">
         <v>284</v>
       </c>
-      <c r="J9" s="6" t="s">
+      <c r="J9" t="s">
         <v>159</v>
       </c>
       <c r="K9" s="1"/>
@@ -6963,7 +6970,7 @@
       <c r="M9" s="1"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="5" t="s">
         <v>36</v>
       </c>
       <c r="B10" t="s">
@@ -6990,7 +6997,7 @@
       <c r="I10" t="s">
         <v>289</v>
       </c>
-      <c r="J10" s="6" t="s">
+      <c r="J10" t="s">
         <v>39</v>
       </c>
       <c r="K10" s="1"/>
@@ -6998,7 +7005,7 @@
       <c r="M10" s="1"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="5" t="s">
         <v>89</v>
       </c>
       <c r="B11" t="s">
@@ -7025,7 +7032,7 @@
       <c r="I11" t="s">
         <v>284</v>
       </c>
-      <c r="J11" s="6" t="s">
+      <c r="J11" t="s">
         <v>94</v>
       </c>
       <c r="K11" s="1"/>
@@ -7033,7 +7040,7 @@
       <c r="M11" s="1"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="5" t="s">
         <v>206</v>
       </c>
       <c r="B12" t="s">
@@ -7060,7 +7067,7 @@
       <c r="I12" t="s">
         <v>280</v>
       </c>
-      <c r="J12" s="6" t="s">
+      <c r="J12" t="s">
         <v>210</v>
       </c>
       <c r="K12" s="1"/>
@@ -7068,7 +7075,7 @@
       <c r="M12" s="1"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="5" t="s">
         <v>217</v>
       </c>
       <c r="B13" t="s">
@@ -7095,7 +7102,7 @@
       <c r="I13" t="s">
         <v>284</v>
       </c>
-      <c r="J13" s="6" t="s">
+      <c r="J13" t="s">
         <v>221</v>
       </c>
       <c r="K13" s="1"/>
@@ -7103,7 +7110,7 @@
       <c r="M13" s="1"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="5" t="s">
         <v>179</v>
       </c>
       <c r="B14" t="s">
@@ -7130,7 +7137,7 @@
       <c r="I14" t="s">
         <v>300</v>
       </c>
-      <c r="J14" s="6" t="s">
+      <c r="J14" t="s">
         <v>183</v>
       </c>
       <c r="K14" s="1"/>
@@ -7138,7 +7145,7 @@
       <c r="M14" s="1"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="5" t="s">
         <v>190</v>
       </c>
       <c r="B15" t="s">
@@ -7165,7 +7172,7 @@
       <c r="I15" t="s">
         <v>280</v>
       </c>
-      <c r="J15" s="6" t="s">
+      <c r="J15" t="s">
         <v>195</v>
       </c>
       <c r="K15" s="1"/>
@@ -7173,7 +7180,7 @@
       <c r="M15" s="1"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="5" t="s">
         <v>110</v>
       </c>
       <c r="B16" t="s">
@@ -7200,7 +7207,7 @@
       <c r="I16" t="s">
         <v>280</v>
       </c>
-      <c r="J16" s="6" t="s">
+      <c r="J16" t="s">
         <v>114</v>
       </c>
       <c r="K16" s="1"/>
@@ -7208,7 +7215,7 @@
       <c r="M16" s="1"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="5" t="s">
         <v>117</v>
       </c>
       <c r="B17" t="s">
@@ -7235,7 +7242,7 @@
       <c r="I17" t="s">
         <v>289</v>
       </c>
-      <c r="J17" s="6" t="s">
+      <c r="J17" t="s">
         <v>120</v>
       </c>
       <c r="K17" s="1"/>
@@ -7243,7 +7250,7 @@
       <c r="M17" s="1"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="5" t="s">
         <v>172</v>
       </c>
       <c r="B18" t="s">
@@ -7270,7 +7277,7 @@
       <c r="I18" t="s">
         <v>280</v>
       </c>
-      <c r="J18" s="6" t="s">
+      <c r="J18" t="s">
         <v>176</v>
       </c>
       <c r="K18" s="1"/>
@@ -7278,7 +7285,7 @@
       <c r="M18" s="1"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="5" t="s">
         <v>122</v>
       </c>
       <c r="B19" t="s">
@@ -7305,7 +7312,7 @@
       <c r="I19" t="s">
         <v>312</v>
       </c>
-      <c r="J19" s="6" t="s">
+      <c r="J19" t="s">
         <v>128</v>
       </c>
       <c r="K19" s="1"/>
@@ -7313,7 +7320,7 @@
       <c r="M19" s="1"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="5" t="s">
         <v>73</v>
       </c>
       <c r="B20" t="s">
@@ -7340,7 +7347,7 @@
       <c r="I20" t="s">
         <v>272</v>
       </c>
-      <c r="J20" s="6" t="s">
+      <c r="J20" t="s">
         <v>78</v>
       </c>
       <c r="K20" s="1"/>
@@ -7348,7 +7355,7 @@
       <c r="M20" s="1"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="5" t="s">
         <v>212</v>
       </c>
       <c r="B21" t="s">
@@ -7375,7 +7382,7 @@
       <c r="I21" t="s">
         <v>318</v>
       </c>
-      <c r="J21" s="6" t="s">
+      <c r="J21" t="s">
         <v>215</v>
       </c>
       <c r="K21" s="1"/>
@@ -7383,7 +7390,7 @@
       <c r="M21" s="1"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="5" t="s">
         <v>167</v>
       </c>
       <c r="B22" t="s">
@@ -7410,7 +7417,7 @@
       <c r="I22" t="s">
         <v>312</v>
       </c>
-      <c r="J22" s="6" t="s">
+      <c r="J22" t="s">
         <v>171</v>
       </c>
       <c r="K22" s="1"/>
@@ -7418,7 +7425,7 @@
       <c r="M22" s="1"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="5" t="s">
         <v>51</v>
       </c>
       <c r="B23" t="s">
@@ -7445,7 +7452,7 @@
       <c r="I23" t="s">
         <v>325</v>
       </c>
-      <c r="J23" s="6" t="s">
+      <c r="J23" t="s">
         <v>54</v>
       </c>
       <c r="K23" s="1"/>
@@ -7453,7 +7460,7 @@
       <c r="M23" s="1"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="5" t="s">
         <v>27</v>
       </c>
       <c r="B24" t="s">
@@ -7480,7 +7487,7 @@
       <c r="I24" t="s">
         <v>280</v>
       </c>
-      <c r="J24" s="6" t="s">
+      <c r="J24" t="s">
         <v>32</v>
       </c>
       <c r="K24" s="1"/>
@@ -7488,7 +7495,7 @@
       <c r="M24" s="1"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="5" t="s">
         <v>184</v>
       </c>
       <c r="B25" t="s">
@@ -7515,7 +7522,7 @@
       <c r="I25" t="s">
         <v>269</v>
       </c>
-      <c r="J25" s="6" t="s">
+      <c r="J25" t="s">
         <v>188</v>
       </c>
       <c r="K25" s="1"/>
@@ -7523,7 +7530,7 @@
       <c r="M25" s="1"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="5" t="s">
         <v>44</v>
       </c>
       <c r="B26" t="s">
@@ -7550,7 +7557,7 @@
       <c r="I26" t="s">
         <v>266</v>
       </c>
-      <c r="J26" s="6" t="s">
+      <c r="J26" t="s">
         <v>48</v>
       </c>
       <c r="K26" s="1"/>
@@ -7558,7 +7565,7 @@
       <c r="M26" s="1"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
+      <c r="A27" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B27" t="s">
@@ -7585,7 +7592,7 @@
       <c r="I27" t="s">
         <v>266</v>
       </c>
-      <c r="J27" s="6" t="s">
+      <c r="J27" t="s">
         <v>21</v>
       </c>
       <c r="K27" s="1"/>
@@ -7593,7 +7600,7 @@
       <c r="M27" s="1"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="5" t="s">
         <v>142</v>
       </c>
       <c r="B28" t="s">
@@ -7620,7 +7627,7 @@
       <c r="I28" t="s">
         <v>336</v>
       </c>
-      <c r="J28" s="6" t="s">
+      <c r="J28" t="s">
         <v>146</v>
       </c>
       <c r="K28" s="1"/>
@@ -7628,7 +7635,7 @@
       <c r="M28" s="1"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="5" t="s">
         <v>83</v>
       </c>
       <c r="B29" t="s">
@@ -7655,7 +7662,7 @@
       <c r="I29" t="s">
         <v>289</v>
       </c>
-      <c r="J29" s="6" t="s">
+      <c r="J29" t="s">
         <v>86</v>
       </c>
       <c r="K29" s="1"/>
@@ -7663,7 +7670,7 @@
       <c r="M29" s="1"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="5" t="s">
         <v>161</v>
       </c>
       <c r="B30" t="s">
@@ -7690,7 +7697,7 @@
       <c r="I30" t="s">
         <v>312</v>
       </c>
-      <c r="J30" s="6" t="s">
+      <c r="J30" t="s">
         <v>165</v>
       </c>
       <c r="K30" s="1"/>
@@ -7756,10 +7763,10 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="7">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="6" t="s">
         <v>197</v>
       </c>
       <c r="C2" s="2">
@@ -7770,10 +7777,10 @@
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="7">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="6" t="s">
         <v>197</v>
       </c>
       <c r="C3" s="2">
@@ -7784,10 +7791,10 @@
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="7">
+      <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="6" t="s">
         <v>137</v>
       </c>
       <c r="C4" s="2">
@@ -7798,10 +7805,10 @@
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
+      <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="6" t="s">
         <v>103</v>
       </c>
       <c r="C5" s="2">
@@ -7812,10 +7819,10 @@
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="7">
+      <c r="A6" s="5">
         <v>5</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="6" t="s">
         <v>63</v>
       </c>
       <c r="C6" s="2">
@@ -7826,10 +7833,10 @@
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="7">
+      <c r="A7" s="5">
         <v>6</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="6" t="s">
         <v>96</v>
       </c>
       <c r="C7" s="2">
@@ -7840,10 +7847,10 @@
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="7">
+      <c r="A8" s="5">
         <v>7</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="6" t="s">
         <v>96</v>
       </c>
       <c r="C8" s="2">
@@ -7854,10 +7861,10 @@
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="7">
+      <c r="A9" s="5">
         <v>8</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="6" t="s">
         <v>132</v>
       </c>
       <c r="C9" s="2">
@@ -7868,10 +7875,10 @@
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
+      <c r="A10" s="5">
         <v>9</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="6" t="s">
         <v>148</v>
       </c>
       <c r="C10" s="2">
@@ -7882,10 +7889,10 @@
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
+      <c r="A11" s="5">
         <v>10</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="6" t="s">
         <v>155</v>
       </c>
       <c r="C11" s="2">
@@ -7896,10 +7903,10 @@
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="7">
+      <c r="A12" s="5">
         <v>11</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="6" t="s">
         <v>36</v>
       </c>
       <c r="C12" s="2">
@@ -7910,10 +7917,10 @@
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="7">
+      <c r="A13" s="5">
         <v>12</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="6" t="s">
         <v>36</v>
       </c>
       <c r="C13" s="2">
@@ -7924,10 +7931,10 @@
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="7">
+      <c r="A14" s="5">
         <v>13</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="6" t="s">
         <v>89</v>
       </c>
       <c r="C14" s="2">
@@ -7938,10 +7945,10 @@
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="7">
+      <c r="A15" s="5">
         <v>14</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="6" t="s">
         <v>206</v>
       </c>
       <c r="C15" s="2">
@@ -7952,10 +7959,10 @@
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="7">
+      <c r="A16" s="5">
         <v>15</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="6" t="s">
         <v>206</v>
       </c>
       <c r="C16" s="2">
@@ -7966,10 +7973,10 @@
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="7">
+      <c r="A17" s="5">
         <v>16</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="6" t="s">
         <v>217</v>
       </c>
       <c r="C17" s="2">
@@ -7980,10 +7987,10 @@
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="7">
+      <c r="A18" s="5">
         <v>17</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="6" t="s">
         <v>179</v>
       </c>
       <c r="C18" s="2">
@@ -7994,10 +8001,10 @@
       <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="7">
+      <c r="A19" s="5">
         <v>18</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="6" t="s">
         <v>190</v>
       </c>
       <c r="C19" s="2">
@@ -8008,10 +8015,10 @@
       <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="7">
+      <c r="A20" s="5">
         <v>19</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="6" t="s">
         <v>110</v>
       </c>
       <c r="C20" s="2">
@@ -8022,10 +8029,10 @@
       <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="7">
+      <c r="A21" s="5">
         <v>20</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="6" t="s">
         <v>117</v>
       </c>
       <c r="C21" s="2">
@@ -8036,10 +8043,10 @@
       <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="7">
+      <c r="A22" s="5">
         <v>21</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="6" t="s">
         <v>172</v>
       </c>
       <c r="C22" s="2">
@@ -8050,10 +8057,10 @@
       <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="7">
+      <c r="A23" s="5">
         <v>22</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="6" t="s">
         <v>172</v>
       </c>
       <c r="C23" s="2">
@@ -8064,10 +8071,10 @@
       <c r="F23" s="1"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="7">
+      <c r="A24" s="5">
         <v>23</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="6" t="s">
         <v>122</v>
       </c>
       <c r="C24" s="2">
@@ -8078,10 +8085,10 @@
       <c r="F24" s="1"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="7">
+      <c r="A25" s="5">
         <v>24</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="6" t="s">
         <v>122</v>
       </c>
       <c r="C25" s="2">
@@ -8092,10 +8099,10 @@
       <c r="F25" s="1"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="7">
+      <c r="A26" s="5">
         <v>25</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="6" t="s">
         <v>73</v>
       </c>
       <c r="C26" s="2">
@@ -8106,10 +8113,10 @@
       <c r="F26" s="1"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="7">
+      <c r="A27" s="5">
         <v>26</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="6" t="s">
         <v>212</v>
       </c>
       <c r="C27" s="2">
@@ -8120,10 +8127,10 @@
       <c r="F27" s="1"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="7">
+      <c r="A28" s="5">
         <v>27</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="6" t="s">
         <v>212</v>
       </c>
       <c r="C28" s="2">
@@ -8134,10 +8141,10 @@
       <c r="F28" s="1"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="7">
+      <c r="A29" s="5">
         <v>28</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="6" t="s">
         <v>167</v>
       </c>
       <c r="C29" s="2">
@@ -8148,10 +8155,10 @@
       <c r="F29" s="1"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="7">
+      <c r="A30" s="5">
         <v>29</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="6" t="s">
         <v>51</v>
       </c>
       <c r="C30" s="2">
@@ -8162,10 +8169,10 @@
       <c r="F30" s="1"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="7">
+      <c r="A31" s="5">
         <v>30</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="6" t="s">
         <v>27</v>
       </c>
       <c r="C31" s="2">
@@ -8176,10 +8183,10 @@
       <c r="F31" s="1"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="7">
+      <c r="A32" s="5">
         <v>31</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="6" t="s">
         <v>184</v>
       </c>
       <c r="C32" s="2">
@@ -8190,10 +8197,10 @@
       <c r="F32" s="1"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="7">
+      <c r="A33" s="5">
         <v>32</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="6" t="s">
         <v>44</v>
       </c>
       <c r="C33" s="2">
@@ -8204,10 +8211,10 @@
       <c r="F33" s="1"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="7">
+      <c r="A34" s="5">
         <v>33</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B34" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C34" s="2">
@@ -8218,10 +8225,10 @@
       <c r="F34" s="1"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="7">
+      <c r="A35" s="5">
         <v>34</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B35" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C35" s="2">
@@ -8232,10 +8239,10 @@
       <c r="F35" s="1"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="7">
+      <c r="A36" s="5">
         <v>35</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B36" s="6" t="s">
         <v>142</v>
       </c>
       <c r="C36" s="2">
@@ -8246,10 +8253,10 @@
       <c r="F36" s="1"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="7">
+      <c r="A37" s="5">
         <v>36</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="B37" s="6" t="s">
         <v>142</v>
       </c>
       <c r="C37" s="2">
@@ -8260,10 +8267,10 @@
       <c r="F37" s="1"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="7">
+      <c r="A38" s="5">
         <v>37</v>
       </c>
-      <c r="B38" s="8" t="s">
+      <c r="B38" s="6" t="s">
         <v>83</v>
       </c>
       <c r="C38" s="2">
@@ -8274,10 +8281,10 @@
       <c r="F38" s="1"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="7">
+      <c r="A39" s="5">
         <v>38</v>
       </c>
-      <c r="B39" s="8" t="s">
+      <c r="B39" s="6" t="s">
         <v>161</v>
       </c>
       <c r="C39" s="2">
@@ -8336,10 +8343,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="13" t="s">
         <v>10</v>
       </c>
       <c r="C1" s="3" t="s">
@@ -8368,10 +8375,10 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="8">
+      <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="6">
         <v>2011</v>
       </c>
       <c r="C2">
@@ -8397,10 +8404,10 @@
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
+      <c r="A3" s="6">
         <v>1</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="6">
         <v>2026</v>
       </c>
       <c r="C3">
@@ -8423,10 +8430,10 @@
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="8">
+      <c r="A4" s="6">
         <v>1</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="6">
         <v>2033</v>
       </c>
       <c r="C4">
@@ -8446,10 +8453,10 @@
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
+      <c r="A5" s="6">
         <v>1</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="6">
         <v>2028</v>
       </c>
       <c r="C5">
@@ -8466,10 +8473,10 @@
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
+      <c r="A6" s="6">
         <v>2</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="6">
         <v>2010</v>
       </c>
       <c r="C6">
@@ -8486,10 +8493,10 @@
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
+      <c r="A7" s="6">
         <v>2</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="6">
         <v>2024</v>
       </c>
       <c r="C7">
@@ -8506,10 +8513,10 @@
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
+      <c r="A8" s="6">
         <v>2</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="6">
         <v>2027</v>
       </c>
       <c r="C8">
@@ -8526,10 +8533,10 @@
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="8">
+      <c r="A9" s="6">
         <v>3</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="6">
         <v>2001</v>
       </c>
       <c r="C9">
@@ -8546,10 +8553,10 @@
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="8">
+      <c r="A10" s="6">
         <v>3</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="6">
         <v>2023</v>
       </c>
       <c r="C10">
@@ -8566,10 +8573,10 @@
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="8">
+      <c r="A11" s="6">
         <v>4</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="6">
         <v>2030</v>
       </c>
       <c r="C11">
@@ -8586,10 +8593,10 @@
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="8">
+      <c r="A12" s="6">
         <v>4</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="6">
         <v>2009</v>
       </c>
       <c r="C12">
@@ -8606,10 +8613,10 @@
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="8">
+      <c r="A13" s="6">
         <v>5</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B13" s="6">
         <v>2010</v>
       </c>
       <c r="C13">
@@ -8626,10 +8633,10 @@
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
+      <c r="A14" s="6">
         <v>5</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B14" s="6">
         <v>2024</v>
       </c>
       <c r="C14">
@@ -8646,10 +8653,10 @@
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="8">
+      <c r="A15" s="6">
         <v>5</v>
       </c>
-      <c r="B15" s="8">
+      <c r="B15" s="6">
         <v>2015</v>
       </c>
       <c r="C15">
@@ -8666,10 +8673,10 @@
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="8">
+      <c r="A16" s="6">
         <v>6</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B16" s="6">
         <v>2004</v>
       </c>
       <c r="C16">
@@ -8686,10 +8693,10 @@
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="8">
+      <c r="A17" s="6">
         <v>6</v>
       </c>
-      <c r="B17" s="8">
+      <c r="B17" s="6">
         <v>2006</v>
       </c>
       <c r="C17">
@@ -8706,10 +8713,10 @@
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="8">
+      <c r="A18" s="6">
         <v>6</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B18" s="6">
         <v>2018</v>
       </c>
       <c r="C18">
@@ -8726,10 +8733,10 @@
       <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="8">
+      <c r="A19" s="6">
         <v>7</v>
       </c>
-      <c r="B19" s="8">
+      <c r="B19" s="6">
         <v>2025</v>
       </c>
       <c r="C19">
@@ -8746,10 +8753,10 @@
       <c r="H19" s="1"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="8">
+      <c r="A20" s="6">
         <v>7</v>
       </c>
-      <c r="B20" s="8">
+      <c r="B20" s="6">
         <v>2010</v>
       </c>
       <c r="C20">
@@ -8766,10 +8773,10 @@
       <c r="H20" s="1"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="8">
+      <c r="A21" s="6">
         <v>7</v>
       </c>
-      <c r="B21" s="8">
+      <c r="B21" s="6">
         <v>2021</v>
       </c>
       <c r="C21">
@@ -8786,10 +8793,10 @@
       <c r="H21" s="1"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="8">
+      <c r="A22" s="6">
         <v>7</v>
       </c>
-      <c r="B22" s="8">
+      <c r="B22" s="6">
         <v>2015</v>
       </c>
       <c r="C22">
@@ -8806,10 +8813,10 @@
       <c r="H22" s="1"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="8">
+      <c r="A23" s="6">
         <v>8</v>
       </c>
-      <c r="B23" s="8">
+      <c r="B23" s="6">
         <v>2004</v>
       </c>
       <c r="C23">
@@ -8826,10 +8833,10 @@
       <c r="H23" s="1"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="8">
+      <c r="A24" s="6">
         <v>8</v>
       </c>
-      <c r="B24" s="8">
+      <c r="B24" s="6">
         <v>2012</v>
       </c>
       <c r="C24">
@@ -8846,10 +8853,10 @@
       <c r="H24" s="1"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="8">
+      <c r="A25" s="6">
         <v>9</v>
       </c>
-      <c r="B25" s="8">
+      <c r="B25" s="6">
         <v>2002</v>
       </c>
       <c r="C25">
@@ -8866,10 +8873,10 @@
       <c r="H25" s="1"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="8">
+      <c r="A26" s="6">
         <v>9</v>
       </c>
-      <c r="B26" s="8">
+      <c r="B26" s="6">
         <v>2026</v>
       </c>
       <c r="C26">
@@ -8886,10 +8893,10 @@
       <c r="H26" s="1"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="8">
+      <c r="A27" s="6">
         <v>9</v>
       </c>
-      <c r="B27" s="8">
+      <c r="B27" s="6">
         <v>2013</v>
       </c>
       <c r="C27">
@@ -8906,10 +8913,10 @@
       <c r="H27" s="1"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="8">
+      <c r="A28" s="6">
         <v>10</v>
       </c>
-      <c r="B28" s="8">
+      <c r="B28" s="6">
         <v>2032</v>
       </c>
       <c r="C28">
@@ -8926,10 +8933,10 @@
       <c r="H28" s="1"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="8">
+      <c r="A29" s="6">
         <v>10</v>
       </c>
-      <c r="B29" s="8">
+      <c r="B29" s="6">
         <v>2020</v>
       </c>
       <c r="C29">
@@ -8946,10 +8953,10 @@
       <c r="H29" s="1"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="8">
+      <c r="A30" s="6">
         <v>11</v>
       </c>
-      <c r="B30" s="8">
+      <c r="B30" s="6">
         <v>2012</v>
       </c>
       <c r="C30">
@@ -8966,10 +8973,10 @@
       <c r="H30" s="1"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="8">
+      <c r="A31" s="6">
         <v>11</v>
       </c>
-      <c r="B31" s="8">
+      <c r="B31" s="6">
         <v>2017</v>
       </c>
       <c r="C31">
@@ -8986,10 +8993,10 @@
       <c r="H31" s="1"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="8">
+      <c r="A32" s="6">
         <v>11</v>
       </c>
-      <c r="B32" s="8">
+      <c r="B32" s="6">
         <v>2016</v>
       </c>
       <c r="C32">
@@ -9006,10 +9013,10 @@
       <c r="H32" s="1"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="8">
+      <c r="A33" s="6">
         <v>12</v>
       </c>
-      <c r="B33" s="8">
+      <c r="B33" s="6">
         <v>2008</v>
       </c>
       <c r="C33">
@@ -9026,10 +9033,10 @@
       <c r="H33" s="1"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="8">
+      <c r="A34" s="6">
         <v>12</v>
       </c>
-      <c r="B34" s="8">
+      <c r="B34" s="6">
         <v>2005</v>
       </c>
       <c r="C34">
@@ -9046,10 +9053,10 @@
       <c r="H34" s="1"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="8">
+      <c r="A35" s="6">
         <v>12</v>
       </c>
-      <c r="B35" s="8">
+      <c r="B35" s="6">
         <v>2019</v>
       </c>
       <c r="C35">
@@ -9066,10 +9073,10 @@
       <c r="H35" s="1"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="8">
+      <c r="A36" s="6">
         <v>13</v>
       </c>
-      <c r="B36" s="8">
+      <c r="B36" s="6">
         <v>2029</v>
       </c>
       <c r="C36">
@@ -9086,10 +9093,10 @@
       <c r="H36" s="1"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="8">
+      <c r="A37" s="6">
         <v>13</v>
       </c>
-      <c r="B37" s="8">
+      <c r="B37" s="6">
         <v>2005</v>
       </c>
       <c r="C37">
@@ -9106,10 +9113,10 @@
       <c r="H37" s="1"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="8">
+      <c r="A38" s="6">
         <v>13</v>
       </c>
-      <c r="B38" s="8">
+      <c r="B38" s="6">
         <v>2022</v>
       </c>
       <c r="C38">
@@ -9126,10 +9133,10 @@
       <c r="H38" s="1"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="8">
+      <c r="A39" s="6">
         <v>14</v>
       </c>
-      <c r="B39" s="8">
+      <c r="B39" s="6">
         <v>2001</v>
       </c>
       <c r="C39">
@@ -9146,10 +9153,10 @@
       <c r="H39" s="1"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="8">
+      <c r="A40" s="6">
         <v>15</v>
       </c>
-      <c r="B40" s="8">
+      <c r="B40" s="6">
         <v>2029</v>
       </c>
       <c r="C40">
@@ -9166,10 +9173,10 @@
       <c r="H40" s="1"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="8">
+      <c r="A41" s="6">
         <v>15</v>
       </c>
-      <c r="B41" s="8">
+      <c r="B41" s="6">
         <v>2011</v>
       </c>
       <c r="C41">
@@ -9186,10 +9193,10 @@
       <c r="H41" s="1"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="8">
+      <c r="A42" s="6">
         <v>15</v>
       </c>
-      <c r="B42" s="8">
+      <c r="B42" s="6">
         <v>2003</v>
       </c>
       <c r="C42">
@@ -9206,10 +9213,10 @@
       <c r="H42" s="1"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="8">
+      <c r="A43" s="6">
         <v>15</v>
       </c>
-      <c r="B43" s="8">
+      <c r="B43" s="6">
         <v>2014</v>
       </c>
       <c r="C43">
@@ -9226,10 +9233,10 @@
       <c r="H43" s="1"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="8">
+      <c r="A44" s="6">
         <v>16</v>
       </c>
-      <c r="B44" s="8">
+      <c r="B44" s="6">
         <v>2007</v>
       </c>
       <c r="C44">
@@ -9246,10 +9253,10 @@
       <c r="H44" s="1"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="8">
+      <c r="A45" s="6">
         <v>16</v>
       </c>
-      <c r="B45" s="8">
+      <c r="B45" s="6">
         <v>2031</v>
       </c>
       <c r="C45">
@@ -9266,10 +9273,10 @@
       <c r="H45" s="1"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="8">
+      <c r="A46" s="6">
         <v>16</v>
       </c>
-      <c r="B46" s="8">
+      <c r="B46" s="6">
         <v>2003</v>
       </c>
       <c r="C46">
@@ -9286,10 +9293,10 @@
       <c r="H46" s="1"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="8">
+      <c r="A47" s="6">
         <v>16</v>
       </c>
-      <c r="B47" s="8">
+      <c r="B47" s="6">
         <v>2020</v>
       </c>
       <c r="C47">
@@ -9306,10 +9313,10 @@
       <c r="H47" s="1"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="8">
+      <c r="A48" s="6">
         <v>17</v>
       </c>
-      <c r="B48" s="8">
+      <c r="B48" s="6">
         <v>2010</v>
       </c>
       <c r="C48">
@@ -9734,7 +9741,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="7">
+      <c r="A2" s="5">
         <v>2001</v>
       </c>
       <c r="B2" t="s">
@@ -9748,7 +9755,7 @@
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="7">
+      <c r="A3" s="5">
         <v>2002</v>
       </c>
       <c r="B3" t="s">
@@ -9762,7 +9769,7 @@
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="7">
+      <c r="A4" s="5">
         <v>2003</v>
       </c>
       <c r="B4" t="s">
@@ -9776,7 +9783,7 @@
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
+      <c r="A5" s="5">
         <v>2004</v>
       </c>
       <c r="B5" t="s">
@@ -9790,7 +9797,7 @@
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="7">
+      <c r="A6" s="5">
         <v>2005</v>
       </c>
       <c r="B6" t="s">
@@ -9804,7 +9811,7 @@
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="7">
+      <c r="A7" s="5">
         <v>2006</v>
       </c>
       <c r="B7" t="s">
@@ -9818,7 +9825,7 @@
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="7">
+      <c r="A8" s="5">
         <v>2007</v>
       </c>
       <c r="B8" t="s">
@@ -9832,7 +9839,7 @@
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="7">
+      <c r="A9" s="5">
         <v>2008</v>
       </c>
       <c r="B9" t="s">
@@ -9846,7 +9853,7 @@
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
+      <c r="A10" s="5">
         <v>2009</v>
       </c>
       <c r="B10" t="s">
@@ -9860,7 +9867,7 @@
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
+      <c r="A11" s="5">
         <v>2010</v>
       </c>
       <c r="B11" t="s">
@@ -9874,7 +9881,7 @@
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="7">
+      <c r="A12" s="5">
         <v>2011</v>
       </c>
       <c r="B12" t="s">
@@ -9888,7 +9895,7 @@
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="7">
+      <c r="A13" s="5">
         <v>2012</v>
       </c>
       <c r="B13" t="s">
@@ -9902,7 +9909,7 @@
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="7">
+      <c r="A14" s="5">
         <v>2013</v>
       </c>
       <c r="B14" t="s">
@@ -9916,7 +9923,7 @@
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="7">
+      <c r="A15" s="5">
         <v>2014</v>
       </c>
       <c r="B15" t="s">
@@ -9930,7 +9937,7 @@
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="7">
+      <c r="A16" s="5">
         <v>2015</v>
       </c>
       <c r="B16" t="s">
@@ -9944,7 +9951,7 @@
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="7">
+      <c r="A17" s="5">
         <v>2016</v>
       </c>
       <c r="B17" t="s">
@@ -9958,7 +9965,7 @@
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="7">
+      <c r="A18" s="5">
         <v>2017</v>
       </c>
       <c r="B18" t="s">
@@ -9972,7 +9979,7 @@
       <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="7">
+      <c r="A19" s="5">
         <v>2018</v>
       </c>
       <c r="B19" t="s">
@@ -9986,7 +9993,7 @@
       <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="7">
+      <c r="A20" s="5">
         <v>2019</v>
       </c>
       <c r="B20" t="s">
@@ -10000,7 +10007,7 @@
       <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="7">
+      <c r="A21" s="5">
         <v>2020</v>
       </c>
       <c r="B21" t="s">
@@ -10014,7 +10021,7 @@
       <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="7">
+      <c r="A22" s="5">
         <v>2021</v>
       </c>
       <c r="B22" t="s">
@@ -10028,7 +10035,7 @@
       <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="7">
+      <c r="A23" s="5">
         <v>2022</v>
       </c>
       <c r="B23" t="s">
@@ -10042,7 +10049,7 @@
       <c r="F23" s="1"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="7">
+      <c r="A24" s="5">
         <v>2023</v>
       </c>
       <c r="B24" t="s">
@@ -10056,7 +10063,7 @@
       <c r="F24" s="1"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="7">
+      <c r="A25" s="5">
         <v>2024</v>
       </c>
       <c r="B25" t="s">
@@ -10070,7 +10077,7 @@
       <c r="F25" s="1"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="7">
+      <c r="A26" s="5">
         <v>2025</v>
       </c>
       <c r="B26" t="s">
@@ -10084,7 +10091,7 @@
       <c r="F26" s="1"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="7">
+      <c r="A27" s="5">
         <v>2026</v>
       </c>
       <c r="B27" t="s">
@@ -10098,7 +10105,7 @@
       <c r="F27" s="1"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="7">
+      <c r="A28" s="5">
         <v>2027</v>
       </c>
       <c r="B28" t="s">
@@ -10112,7 +10119,7 @@
       <c r="F28" s="1"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="7">
+      <c r="A29" s="5">
         <v>2028</v>
       </c>
       <c r="B29" t="s">
@@ -10126,7 +10133,7 @@
       <c r="F29" s="1"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="7">
+      <c r="A30" s="5">
         <v>2029</v>
       </c>
       <c r="B30" t="s">
@@ -10140,7 +10147,7 @@
       <c r="F30" s="1"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="7">
+      <c r="A31" s="5">
         <v>2030</v>
       </c>
       <c r="B31" t="s">
@@ -10154,7 +10161,7 @@
       <c r="F31" s="1"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="7">
+      <c r="A32" s="5">
         <v>2031</v>
       </c>
       <c r="B32" t="s">
@@ -10168,7 +10175,7 @@
       <c r="F32" s="1"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="7">
+      <c r="A33" s="5">
         <v>2032</v>
       </c>
       <c r="B33" t="s">
@@ -10182,7 +10189,7 @@
       <c r="F33" s="1"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="7">
+      <c r="A34" s="5">
         <v>2033</v>
       </c>
       <c r="B34" t="s">
@@ -10513,238 +10520,262 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7947388-8A49-411E-9DD7-B487EF261802}">
-  <dimension ref="B2:E20"/>
+  <dimension ref="B2:K20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.85546875" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="11" t="s">
+    <row r="2" spans="2:11" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="16" t="s">
         <v>364</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-    </row>
-    <row r="3" spans="2:5" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="10" t="s">
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+    </row>
+    <row r="3" spans="2:11" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="8" t="s">
+        <v>423</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>344</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="D3" s="8" t="s">
         <v>345</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="E3" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="F3" s="8" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="4" spans="2:5" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="13" t="s">
+    <row r="4" spans="2:11" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="19">
+        <v>1</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>347</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="D4" s="10" t="s">
         <v>353</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="E4" s="10" t="s">
         <v>359</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="F4" s="10" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="5" spans="2:5" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="13" t="s">
+    <row r="5" spans="2:11" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="19">
+        <v>2</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>346</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="D5" s="10" t="s">
         <v>354</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="E5" s="10" t="s">
         <v>361</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="F5" s="10" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="6" spans="2:5" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="13" t="s">
+    <row r="6" spans="2:11" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="19">
+        <v>3</v>
+      </c>
+      <c r="C6" s="10" t="s">
         <v>348</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="D6" s="10" t="s">
         <v>355</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="E6" s="10" t="s">
         <v>361</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="F6" s="10" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="7" spans="2:5" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="13" t="s">
+    <row r="7" spans="2:11" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="19">
+        <v>4</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>349</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="D7" s="10" t="s">
         <v>356</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="E7" s="10" t="s">
         <v>359</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="F7" s="10" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="8" spans="2:5" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="13" t="s">
+    <row r="8" spans="2:11" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="19">
+        <v>5</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>350</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="D8" s="10" t="s">
         <v>353</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="E8" s="10" t="s">
         <v>361</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="F8" s="10" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="9" spans="2:5" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="13" t="s">
+      <c r="K8" s="18"/>
+    </row>
+    <row r="9" spans="2:11" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="19">
+        <v>6</v>
+      </c>
+      <c r="C9" s="10" t="s">
         <v>352</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="D9" s="10" t="s">
         <v>354</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="E9" s="10" t="s">
         <v>360</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="F9" s="10" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="13" spans="2:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="11" t="s">
+    <row r="13" spans="2:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="16" t="s">
         <v>364</v>
       </c>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-    </row>
-    <row r="14" spans="2:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="10" t="s">
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+    </row>
+    <row r="14" spans="2:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="8" t="s">
         <v>344</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="D14" s="8" t="s">
         <v>345</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="E14" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="F14" s="8" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="15" spans="2:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="13" t="s">
+    <row r="15" spans="2:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="10" t="s">
         <v>348</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="D15" s="10" t="s">
         <v>355</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="E15" s="10" t="s">
         <v>361</v>
       </c>
-      <c r="E15" s="13" t="s">
+      <c r="F15" s="10" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="16" spans="2:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="13" t="s">
+    <row r="16" spans="2:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="10" t="s">
         <v>347</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="D16" s="10" t="s">
         <v>353</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="E16" s="10" t="s">
         <v>359</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="F16" s="10" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="17" spans="2:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="13" t="s">
+    <row r="17" spans="3:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="10" t="s">
         <v>350</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="D17" s="10" t="s">
         <v>353</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="E17" s="10" t="s">
         <v>361</v>
       </c>
-      <c r="E17" s="13" t="s">
+      <c r="F17" s="10" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="18" spans="2:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="13" t="s">
+    <row r="18" spans="3:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="10" t="s">
         <v>346</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="D18" s="10" t="s">
         <v>354</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="E18" s="10" t="s">
         <v>361</v>
       </c>
-      <c r="E18" s="13" t="s">
+      <c r="F18" s="10" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="19" spans="2:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="13" t="s">
+    <row r="19" spans="3:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="10" t="s">
         <v>352</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="D19" s="10" t="s">
         <v>354</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="E19" s="10" t="s">
         <v>360</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="F19" s="10" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="20" spans="2:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="13" t="s">
+    <row r="20" spans="3:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C20" s="10" t="s">
         <v>349</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="D20" s="10" t="s">
         <v>356</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="E20" s="10" t="s">
         <v>359</v>
       </c>
-      <c r="E20" s="13" t="s">
+      <c r="F20" s="10" t="s">
         <v>358</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B15:E20">
-    <sortCondition ref="C15:C20"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C15:F20">
+    <sortCondition ref="D15:D20"/>
   </sortState>
   <mergeCells count="2">
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="B2:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -10755,732 +10786,732 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05E766EB-821B-4618-B2CF-8F6F3BC20E3B}">
   <dimension ref="B2:Y21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="M1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="9"/>
-    <col min="2" max="2" width="13.140625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" style="9" customWidth="1"/>
-    <col min="4" max="4" width="26.7109375" style="9" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="9"/>
-    <col min="6" max="6" width="25.42578125" style="9" customWidth="1"/>
-    <col min="7" max="7" width="17" style="9" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" style="9" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="9"/>
-    <col min="10" max="13" width="24.7109375" style="9" customWidth="1"/>
-    <col min="14" max="15" width="9.140625" style="9"/>
-    <col min="16" max="16" width="14.42578125" style="9" customWidth="1"/>
-    <col min="17" max="17" width="22" style="9" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.42578125" style="9" customWidth="1"/>
-    <col min="19" max="19" width="9.140625" style="9"/>
-    <col min="20" max="21" width="16.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.28515625" style="9" customWidth="1"/>
-    <col min="23" max="23" width="9.140625" style="9"/>
-    <col min="24" max="24" width="18.28515625" style="9" customWidth="1"/>
-    <col min="25" max="25" width="16" style="9" customWidth="1"/>
-    <col min="26" max="16384" width="9.140625" style="9"/>
+    <col min="1" max="1" width="9.140625" style="7"/>
+    <col min="2" max="2" width="13.140625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" style="7" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="7"/>
+    <col min="6" max="6" width="25.42578125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="17" style="7" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" style="7" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="7"/>
+    <col min="10" max="13" width="24.7109375" style="7" customWidth="1"/>
+    <col min="14" max="15" width="9.140625" style="7"/>
+    <col min="16" max="16" width="14.42578125" style="7" customWidth="1"/>
+    <col min="17" max="17" width="22" style="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.42578125" style="7" customWidth="1"/>
+    <col min="19" max="19" width="9.140625" style="7"/>
+    <col min="20" max="21" width="16.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.28515625" style="7" customWidth="1"/>
+    <col min="23" max="23" width="9.140625" style="7"/>
+    <col min="24" max="24" width="18.28515625" style="7" customWidth="1"/>
+    <col min="25" max="25" width="16" style="7" customWidth="1"/>
+    <col min="26" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:25" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="17" t="s">
         <v>404</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="P2" s="19" t="s">
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="P2" s="15" t="s">
         <v>420</v>
       </c>
-      <c r="X2" s="19" t="s">
+      <c r="X2" s="15" t="s">
         <v>419</v>
       </c>
     </row>
     <row r="3" spans="2:25" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="12" t="s">
         <v>365</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="12" t="s">
         <v>366</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="12" t="s">
         <v>374</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="12" t="s">
         <v>383</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="12" t="s">
         <v>375</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="G3" s="12" t="s">
         <v>392</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="12" t="s">
         <v>403</v>
       </c>
-      <c r="P3" s="15" t="s">
+      <c r="P3" s="12" t="s">
         <v>414</v>
       </c>
-      <c r="Q3" s="15" t="s">
+      <c r="Q3" s="12" t="s">
         <v>417</v>
       </c>
-      <c r="R3" s="15" t="s">
+      <c r="R3" s="12" t="s">
         <v>406</v>
       </c>
-      <c r="S3" s="15" t="s">
+      <c r="S3" s="12" t="s">
         <v>383</v>
       </c>
-      <c r="T3" s="15" t="s">
+      <c r="T3" s="12" t="s">
         <v>415</v>
       </c>
-      <c r="U3" s="15" t="s">
+      <c r="U3" s="12" t="s">
         <v>416</v>
       </c>
-      <c r="V3" s="15" t="s">
+      <c r="V3" s="12" t="s">
         <v>422</v>
       </c>
-      <c r="X3" s="15" t="s">
+      <c r="X3" s="12" t="s">
         <v>405</v>
       </c>
-      <c r="Y3" s="15" t="s">
+      <c r="Y3" s="12" t="s">
         <v>414</v>
       </c>
     </row>
     <row r="4" spans="2:25" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="11" t="s">
         <v>351</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="11" t="s">
         <v>357</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="11" t="s">
         <v>376</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="11" t="s">
         <v>379</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="11" t="s">
         <v>391</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="11" t="s">
         <v>393</v>
       </c>
-      <c r="H4" s="14">
+      <c r="H4" s="11">
         <v>20</v>
       </c>
-      <c r="P4" s="14">
+      <c r="P4" s="11">
         <v>301</v>
       </c>
-      <c r="Q4" s="14" t="s">
+      <c r="Q4" s="11" t="s">
         <v>376</v>
       </c>
-      <c r="R4" s="14">
+      <c r="R4" s="11">
         <v>201</v>
       </c>
-      <c r="S4" s="14" t="s">
+      <c r="S4" s="11" t="s">
         <v>379</v>
       </c>
-      <c r="T4" s="18">
+      <c r="T4" s="14">
         <v>0.70833333333333337</v>
       </c>
-      <c r="U4" s="18">
+      <c r="U4" s="14">
         <v>0.75</v>
       </c>
-      <c r="V4" s="14">
+      <c r="V4" s="11">
         <v>20</v>
       </c>
-      <c r="X4" s="14">
+      <c r="X4" s="11">
         <v>101</v>
       </c>
-      <c r="Y4" s="14">
+      <c r="Y4" s="11">
         <v>301</v>
       </c>
     </row>
     <row r="5" spans="2:25" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="11" t="s">
         <v>347</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="11" t="s">
         <v>367</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="11" t="s">
         <v>385</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="11" t="s">
         <v>380</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="11" t="s">
         <v>389</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="11" t="s">
         <v>394</v>
       </c>
-      <c r="H5" s="14">
+      <c r="H5" s="11">
         <v>45</v>
       </c>
-      <c r="P5" s="14">
+      <c r="P5" s="11">
         <v>302</v>
       </c>
-      <c r="Q5" s="14" t="s">
+      <c r="Q5" s="11" t="s">
         <v>385</v>
       </c>
-      <c r="R5" s="14">
+      <c r="R5" s="11">
         <v>202</v>
       </c>
-      <c r="S5" s="14" t="s">
+      <c r="S5" s="11" t="s">
         <v>380</v>
       </c>
-      <c r="T5" s="18">
+      <c r="T5" s="14">
         <v>0.25</v>
       </c>
-      <c r="U5" s="18">
+      <c r="U5" s="14">
         <v>0.3125</v>
       </c>
-      <c r="V5" s="14">
+      <c r="V5" s="11">
         <v>45</v>
       </c>
-      <c r="X5" s="14">
+      <c r="X5" s="11">
         <v>102</v>
       </c>
-      <c r="Y5" s="14">
+      <c r="Y5" s="11">
         <v>302</v>
       </c>
     </row>
     <row r="6" spans="2:25" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="11" t="s">
         <v>368</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="11" t="s">
         <v>369</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="11" t="s">
         <v>396</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="11" t="s">
         <v>380</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="11" t="s">
         <v>388</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="G6" s="11" t="s">
         <v>395</v>
       </c>
-      <c r="H6" s="14">
+      <c r="H6" s="11">
         <v>30</v>
       </c>
-      <c r="P6" s="14">
+      <c r="P6" s="11">
         <v>303</v>
       </c>
-      <c r="Q6" s="14" t="s">
+      <c r="Q6" s="11" t="s">
         <v>396</v>
       </c>
-      <c r="R6" s="14">
+      <c r="R6" s="11">
         <v>203</v>
       </c>
-      <c r="S6" s="14" t="s">
+      <c r="S6" s="11" t="s">
         <v>380</v>
       </c>
-      <c r="T6" s="18">
+      <c r="T6" s="14">
         <v>0.77083333333333337</v>
       </c>
-      <c r="U6" s="18">
+      <c r="U6" s="14">
         <v>0.8125</v>
       </c>
-      <c r="V6" s="14">
+      <c r="V6" s="11">
         <v>30</v>
       </c>
-      <c r="X6" s="14">
+      <c r="X6" s="11">
         <v>103</v>
       </c>
-      <c r="Y6" s="14">
+      <c r="Y6" s="11">
         <v>303</v>
       </c>
     </row>
     <row r="7" spans="2:25" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="11" t="s">
         <v>370</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="11" t="s">
         <v>371</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="11" t="s">
         <v>377</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="11" t="s">
         <v>380</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="11" t="s">
         <v>387</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="G7" s="11" t="s">
         <v>399</v>
       </c>
-      <c r="H7" s="14">
+      <c r="H7" s="11">
         <v>30</v>
       </c>
-      <c r="P7" s="14">
+      <c r="P7" s="11">
         <v>304</v>
       </c>
-      <c r="Q7" s="14" t="s">
+      <c r="Q7" s="11" t="s">
         <v>377</v>
       </c>
-      <c r="R7" s="14">
+      <c r="R7" s="11">
         <v>204</v>
       </c>
-      <c r="S7" s="14" t="s">
+      <c r="S7" s="11" t="s">
         <v>380</v>
       </c>
-      <c r="T7" s="18">
+      <c r="T7" s="14">
         <v>0.33333333333333331</v>
       </c>
-      <c r="U7" s="18">
+      <c r="U7" s="14">
         <v>0.375</v>
       </c>
-      <c r="V7" s="14">
+      <c r="V7" s="11">
         <v>30</v>
       </c>
-      <c r="X7" s="14">
+      <c r="X7" s="11">
         <v>104</v>
       </c>
-      <c r="Y7" s="14">
+      <c r="Y7" s="11">
         <v>304</v>
       </c>
     </row>
     <row r="8" spans="2:25" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="11" t="s">
         <v>372</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="11" t="s">
         <v>373</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="11" t="s">
         <v>378</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="11" t="s">
         <v>381</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="11" t="s">
         <v>389</v>
       </c>
-      <c r="G8" s="14" t="s">
+      <c r="G8" s="11" t="s">
         <v>398</v>
       </c>
-      <c r="H8" s="14">
+      <c r="H8" s="11">
         <v>15</v>
       </c>
-      <c r="P8" s="14">
+      <c r="P8" s="11">
         <v>305</v>
       </c>
-      <c r="Q8" s="14" t="s">
+      <c r="Q8" s="11" t="s">
         <v>378</v>
       </c>
-      <c r="R8" s="14">
+      <c r="R8" s="11">
         <v>202</v>
       </c>
-      <c r="S8" s="14" t="s">
+      <c r="S8" s="11" t="s">
         <v>381</v>
       </c>
-      <c r="T8" s="18">
+      <c r="T8" s="14">
         <v>0.5</v>
       </c>
-      <c r="U8" s="18">
+      <c r="U8" s="14">
         <v>0.53125</v>
       </c>
-      <c r="V8" s="14">
+      <c r="V8" s="11">
         <v>15</v>
       </c>
-      <c r="X8" s="14">
+      <c r="X8" s="11">
         <v>105</v>
       </c>
-      <c r="Y8" s="14">
+      <c r="Y8" s="11">
         <v>305</v>
       </c>
     </row>
     <row r="9" spans="2:25" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="11" t="s">
         <v>347</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="11" t="s">
         <v>367</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="11" t="s">
         <v>397</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="11" t="s">
         <v>379</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="11" t="s">
         <v>388</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="G9" s="11" t="s">
         <v>395</v>
       </c>
-      <c r="H9" s="14">
+      <c r="H9" s="11">
         <v>20</v>
       </c>
-      <c r="P9" s="14">
+      <c r="P9" s="11">
         <v>306</v>
       </c>
-      <c r="Q9" s="14" t="s">
+      <c r="Q9" s="11" t="s">
         <v>397</v>
       </c>
-      <c r="R9" s="14">
+      <c r="R9" s="11">
         <v>203</v>
       </c>
-      <c r="S9" s="14" t="s">
+      <c r="S9" s="11" t="s">
         <v>379</v>
       </c>
-      <c r="T9" s="18">
+      <c r="T9" s="14">
         <v>0.77083333333333337</v>
       </c>
-      <c r="U9" s="18">
+      <c r="U9" s="14">
         <v>0.8125</v>
       </c>
-      <c r="V9" s="14">
+      <c r="V9" s="11">
         <v>20</v>
       </c>
-      <c r="X9" s="14">
+      <c r="X9" s="11">
         <v>102</v>
       </c>
-      <c r="Y9" s="14">
+      <c r="Y9" s="11">
         <v>306</v>
       </c>
     </row>
     <row r="10" spans="2:25" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="11" t="s">
         <v>372</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="11" t="s">
         <v>373</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="11" t="s">
         <v>396</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="11" t="s">
         <v>380</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="F10" s="11" t="s">
         <v>388</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="G10" s="11" t="s">
         <v>395</v>
       </c>
-      <c r="H10" s="14">
+      <c r="H10" s="11">
         <v>30</v>
       </c>
-      <c r="P10" s="14">
+      <c r="P10" s="11">
         <v>307</v>
       </c>
-      <c r="Q10" s="14" t="s">
+      <c r="Q10" s="11" t="s">
         <v>382</v>
       </c>
-      <c r="R10" s="14">
+      <c r="R10" s="11">
         <v>204</v>
       </c>
-      <c r="S10" s="14" t="s">
+      <c r="S10" s="11" t="s">
         <v>379</v>
       </c>
-      <c r="T10" s="18">
+      <c r="T10" s="14">
         <v>0.33333333333333331</v>
       </c>
-      <c r="U10" s="18">
+      <c r="U10" s="14">
         <v>0.375</v>
       </c>
-      <c r="V10" s="14">
+      <c r="V10" s="11">
         <v>20</v>
       </c>
-      <c r="X10" s="14">
+      <c r="X10" s="11">
         <v>105</v>
       </c>
-      <c r="Y10" s="14">
+      <c r="Y10" s="11">
         <v>303</v>
       </c>
     </row>
     <row r="11" spans="2:25" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="11" t="s">
         <v>368</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="11" t="s">
         <v>369</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="11" t="s">
         <v>382</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="11" t="s">
         <v>379</v>
       </c>
-      <c r="F11" s="14" t="s">
+      <c r="F11" s="11" t="s">
         <v>387</v>
       </c>
-      <c r="G11" s="14" t="s">
+      <c r="G11" s="11" t="s">
         <v>399</v>
       </c>
-      <c r="H11" s="14">
+      <c r="H11" s="11">
         <v>20</v>
       </c>
-      <c r="P11" s="14">
+      <c r="P11" s="11">
         <v>308</v>
       </c>
-      <c r="Q11" s="14" t="s">
+      <c r="Q11" s="11" t="s">
         <v>386</v>
       </c>
-      <c r="R11" s="14">
+      <c r="R11" s="11">
         <v>205</v>
       </c>
-      <c r="S11" s="14" t="s">
+      <c r="S11" s="11" t="s">
         <v>379</v>
       </c>
-      <c r="T11" s="18">
+      <c r="T11" s="14">
         <v>0.83333333333333337</v>
       </c>
-      <c r="U11" s="18">
+      <c r="U11" s="14">
         <v>0.875</v>
       </c>
-      <c r="V11" s="14">
+      <c r="V11" s="11">
         <v>20</v>
       </c>
-      <c r="X11" s="14">
+      <c r="X11" s="11">
         <v>103</v>
       </c>
-      <c r="Y11" s="14">
+      <c r="Y11" s="11">
         <v>307</v>
       </c>
     </row>
     <row r="12" spans="2:25" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="11" t="s">
         <v>351</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="11" t="s">
         <v>357</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="11" t="s">
         <v>385</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="11" t="s">
         <v>380</v>
       </c>
-      <c r="F12" s="14" t="s">
+      <c r="F12" s="11" t="s">
         <v>389</v>
       </c>
-      <c r="G12" s="14" t="s">
+      <c r="G12" s="11" t="s">
         <v>394</v>
       </c>
-      <c r="H12" s="14">
+      <c r="H12" s="11">
         <v>45</v>
       </c>
-      <c r="X12" s="14">
+      <c r="X12" s="11">
         <v>101</v>
       </c>
-      <c r="Y12" s="14">
+      <c r="Y12" s="11">
         <v>302</v>
       </c>
     </row>
     <row r="13" spans="2:25" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="11" t="s">
         <v>384</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="11" t="s">
         <v>353</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="11" t="s">
         <v>386</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="11" t="s">
         <v>379</v>
       </c>
-      <c r="F13" s="14" t="s">
+      <c r="F13" s="11" t="s">
         <v>390</v>
       </c>
-      <c r="G13" s="14" t="s">
+      <c r="G13" s="11" t="s">
         <v>400</v>
       </c>
-      <c r="H13" s="14">
+      <c r="H13" s="11">
         <v>20</v>
       </c>
-      <c r="P13" s="19" t="s">
+      <c r="P13" s="15" t="s">
         <v>421</v>
       </c>
-      <c r="T13" s="19" t="s">
+      <c r="T13" s="15" t="s">
         <v>418</v>
       </c>
-      <c r="X13" s="14">
+      <c r="X13" s="11">
         <v>106</v>
       </c>
-      <c r="Y13" s="14">
+      <c r="Y13" s="11">
         <v>308</v>
       </c>
     </row>
     <row r="14" spans="2:25" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="11" t="s">
         <v>401</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="11" t="s">
         <v>402</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="11" t="s">
         <v>377</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E14" s="11" t="s">
         <v>380</v>
       </c>
-      <c r="F14" s="14" t="s">
+      <c r="F14" s="11" t="s">
         <v>387</v>
       </c>
-      <c r="G14" s="14" t="s">
+      <c r="G14" s="11" t="s">
         <v>399</v>
       </c>
-      <c r="H14" s="14">
+      <c r="H14" s="11">
         <v>30</v>
       </c>
-      <c r="P14" s="15" t="s">
+      <c r="P14" s="12" t="s">
         <v>406</v>
       </c>
-      <c r="Q14" s="15" t="s">
+      <c r="Q14" s="12" t="s">
         <v>365</v>
       </c>
-      <c r="R14" s="15" t="s">
+      <c r="R14" s="12" t="s">
         <v>366</v>
       </c>
-      <c r="T14" s="15" t="s">
+      <c r="T14" s="12" t="s">
         <v>405</v>
       </c>
-      <c r="U14" s="15" t="s">
+      <c r="U14" s="12" t="s">
         <v>365</v>
       </c>
-      <c r="V14" s="15" t="s">
+      <c r="V14" s="12" t="s">
         <v>366</v>
       </c>
-      <c r="X14" s="14">
+      <c r="X14" s="11">
         <v>107</v>
       </c>
-      <c r="Y14" s="14">
+      <c r="Y14" s="11">
         <v>304</v>
       </c>
     </row>
     <row r="15" spans="2:25" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P15" s="14">
+      <c r="P15" s="11">
         <v>201</v>
       </c>
-      <c r="Q15" s="14" t="s">
+      <c r="Q15" s="11" t="s">
         <v>411</v>
       </c>
-      <c r="R15" s="14" t="s">
+      <c r="R15" s="11" t="s">
         <v>407</v>
       </c>
-      <c r="T15" s="14">
+      <c r="T15" s="11">
         <v>101</v>
       </c>
-      <c r="U15" s="14" t="s">
+      <c r="U15" s="11" t="s">
         <v>351</v>
       </c>
-      <c r="V15" s="14" t="s">
+      <c r="V15" s="11" t="s">
         <v>357</v>
       </c>
     </row>
     <row r="16" spans="2:25" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P16" s="14">
+      <c r="P16" s="11">
         <v>202</v>
       </c>
-      <c r="Q16" s="14" t="s">
+      <c r="Q16" s="11" t="s">
         <v>412</v>
       </c>
-      <c r="R16" s="14" t="s">
+      <c r="R16" s="11" t="s">
         <v>408</v>
       </c>
-      <c r="T16" s="14">
+      <c r="T16" s="11">
         <v>102</v>
       </c>
-      <c r="U16" s="14" t="s">
+      <c r="U16" s="11" t="s">
         <v>347</v>
       </c>
-      <c r="V16" s="14" t="s">
+      <c r="V16" s="11" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="17" spans="16:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P17" s="14">
+      <c r="P17" s="11">
         <v>203</v>
       </c>
-      <c r="Q17" s="14" t="s">
+      <c r="Q17" s="11" t="s">
         <v>413</v>
       </c>
-      <c r="R17" s="14" t="s">
+      <c r="R17" s="11" t="s">
         <v>409</v>
       </c>
-      <c r="T17" s="14">
+      <c r="T17" s="11">
         <v>103</v>
       </c>
-      <c r="U17" s="14" t="s">
+      <c r="U17" s="11" t="s">
         <v>368</v>
       </c>
-      <c r="V17" s="14" t="s">
+      <c r="V17" s="11" t="s">
         <v>369</v>
       </c>
     </row>
     <row r="18" spans="16:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P18" s="14">
+      <c r="P18" s="11">
         <v>204</v>
       </c>
-      <c r="Q18" s="14" t="s">
+      <c r="Q18" s="11" t="s">
         <v>352</v>
       </c>
-      <c r="R18" s="14" t="s">
+      <c r="R18" s="11" t="s">
         <v>410</v>
       </c>
-      <c r="T18" s="14">
+      <c r="T18" s="11">
         <v>104</v>
       </c>
-      <c r="U18" s="14" t="s">
+      <c r="U18" s="11" t="s">
         <v>370</v>
       </c>
-      <c r="V18" s="14" t="s">
+      <c r="V18" s="11" t="s">
         <v>371</v>
       </c>
     </row>
     <row r="19" spans="16:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P19" s="14">
+      <c r="P19" s="11">
         <v>205</v>
       </c>
-      <c r="Q19" s="14" t="s">
+      <c r="Q19" s="11" t="s">
         <v>346</v>
       </c>
-      <c r="R19" s="14" t="s">
+      <c r="R19" s="11" t="s">
         <v>356</v>
       </c>
-      <c r="T19" s="14">
+      <c r="T19" s="11">
         <v>105</v>
       </c>
-      <c r="U19" s="14" t="s">
+      <c r="U19" s="11" t="s">
         <v>372</v>
       </c>
-      <c r="V19" s="14" t="s">
+      <c r="V19" s="11" t="s">
         <v>373</v>
       </c>
     </row>
     <row r="20" spans="16:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="T20" s="14">
+      <c r="T20" s="11">
         <v>106</v>
       </c>
-      <c r="U20" s="14" t="s">
+      <c r="U20" s="11" t="s">
         <v>384</v>
       </c>
-      <c r="V20" s="14" t="s">
+      <c r="V20" s="11" t="s">
         <v>353</v>
       </c>
     </row>
     <row r="21" spans="16:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="T21" s="14">
+      <c r="T21" s="11">
         <v>107</v>
       </c>
-      <c r="U21" s="14" t="s">
+      <c r="U21" s="11" t="s">
         <v>401</v>
       </c>
-      <c r="V21" s="14" t="s">
+      <c r="V21" s="11" t="s">
         <v>402</v>
       </c>
     </row>

</xml_diff>